<commit_message>
Fixed Los Angeles Clippers & Miami Heat Logic
</commit_message>
<xml_diff>
--- a/nba_elo_tracker.xlsx
+++ b/nba_elo_tracker.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.############"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>1794.86</v>
+        <v>1797.1</v>
       </c>
     </row>
     <row r="6">
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>1774.79</v>
+        <v>1777.48</v>
       </c>
     </row>
     <row r="7">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>1683.63</v>
+        <v>1683.9</v>
       </c>
     </row>
     <row r="8">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="C8" s="3" t="n">
-        <v>1661.31</v>
+        <v>1661.8</v>
       </c>
     </row>
     <row r="9">
@@ -583,7 +583,7 @@
         </is>
       </c>
       <c r="C9" s="3" t="n">
-        <v>1616.27</v>
+        <v>1616.82</v>
       </c>
     </row>
     <row r="10">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="C10" s="3" t="n">
-        <v>1611.84</v>
+        <v>1612.74</v>
       </c>
     </row>
     <row r="11">
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>1601.66</v>
+        <v>1601.3</v>
       </c>
     </row>
     <row r="12">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="C12" s="3" t="n">
-        <v>1589.16</v>
+        <v>1589.98</v>
       </c>
     </row>
     <row r="13">
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="C13" s="3" t="n">
-        <v>1587.9</v>
+        <v>1588.03</v>
       </c>
     </row>
     <row r="14">
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="C14" s="3" t="n">
-        <v>1582.42</v>
+        <v>1582.82</v>
       </c>
     </row>
     <row r="15">
@@ -661,7 +661,7 @@
         </is>
       </c>
       <c r="C15" s="3" t="n">
-        <v>1578.2</v>
+        <v>1578.14</v>
       </c>
     </row>
     <row r="16">
@@ -674,7 +674,7 @@
         </is>
       </c>
       <c r="C16" s="3" t="n">
-        <v>1552.24</v>
+        <v>1551.64</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" s="3" t="n">
-        <v>1542.08</v>
+        <v>1541.98</v>
       </c>
     </row>
     <row r="18">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="C18" s="3" t="n">
-        <v>1528.65</v>
+        <v>1529.16</v>
       </c>
     </row>
     <row r="19">
@@ -713,7 +713,7 @@
         </is>
       </c>
       <c r="C19" s="3" t="n">
-        <v>1502.91</v>
+        <v>1502.88</v>
       </c>
     </row>
     <row r="20">
@@ -722,11 +722,11 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Los Angeles Clippers</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="C20" s="3" t="n">
-        <v>1500</v>
+        <v>1478.74</v>
       </c>
     </row>
     <row r="21">
@@ -735,11 +735,11 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Dallas Mavericks</t>
+          <t>Los Angeles Clippers</t>
         </is>
       </c>
       <c r="C21" s="3" t="n">
-        <v>1478.46</v>
+        <v>1470.47</v>
       </c>
     </row>
     <row r="22">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="C22" s="3" t="n">
-        <v>1465.9</v>
+        <v>1465.62</v>
       </c>
     </row>
     <row r="23">
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="C23" s="3" t="n">
-        <v>1438.57</v>
+        <v>1438.25</v>
       </c>
     </row>
     <row r="24">
@@ -778,7 +778,7 @@
         </is>
       </c>
       <c r="C24" s="3" t="n">
-        <v>1438.32</v>
+        <v>1438.01</v>
       </c>
     </row>
     <row r="25">
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="C25" s="3" t="n">
-        <v>1437.44</v>
+        <v>1436.24</v>
       </c>
     </row>
     <row r="26">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="C27" s="3" t="n">
-        <v>1388.6</v>
+        <v>1388.17</v>
       </c>
     </row>
     <row r="28">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="C28" s="3" t="n">
-        <v>1379.1</v>
+        <v>1378.24</v>
       </c>
     </row>
     <row r="29">
@@ -843,7 +843,7 @@
         </is>
       </c>
       <c r="C29" s="3" t="n">
-        <v>1358.66</v>
+        <v>1358.1</v>
       </c>
     </row>
     <row r="30">
@@ -856,7 +856,7 @@
         </is>
       </c>
       <c r="C30" s="3" t="n">
-        <v>1356.21</v>
+        <v>1355.48</v>
       </c>
     </row>
     <row r="31">
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="C31" s="3" t="n">
-        <v>1326.34</v>
+        <v>1325.78</v>
       </c>
     </row>
     <row r="32">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="C32" s="3" t="n">
-        <v>1285.95</v>
+        <v>1285.63</v>
       </c>
     </row>
     <row r="33">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="C33" s="3" t="n">
-        <v>1278.6</v>
+        <v>1277.19</v>
       </c>
     </row>
     <row r="34">
@@ -908,7 +908,7 @@
         </is>
       </c>
       <c r="C34" s="3" t="n">
-        <v>1263.9</v>
+        <v>1262.75</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1"/>
@@ -963,10 +963,10 @@
         </is>
       </c>
       <c r="C39" s="3" t="n">
-        <v>1794.86</v>
+        <v>1797.1</v>
       </c>
       <c r="D39" s="3" t="n">
-        <v>1356.21</v>
+        <v>1355.48</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="F39" s="4" t="n">
-        <v>0.9569223789705138</v>
+        <v>0.9576216581651262</v>
       </c>
     </row>
     <row r="40">
@@ -989,10 +989,10 @@
         </is>
       </c>
       <c r="C40" s="3" t="n">
-        <v>1578.2</v>
+        <v>1578.14</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>1278.6</v>
+        <v>1277.19</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="F40" s="4" t="n">
-        <v>0.9089004334647053</v>
+        <v>0.9095418528145847</v>
       </c>
     </row>
     <row r="41">
@@ -1015,10 +1015,10 @@
         </is>
       </c>
       <c r="C41" s="3" t="n">
-        <v>1552.24</v>
+        <v>1551.64</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>1542.08</v>
+        <v>1541.98</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="F41" s="4" t="n">
-        <v>0.6534257745402825</v>
+        <v>0.6527736812238141</v>
       </c>
     </row>
     <row r="42">
@@ -1041,10 +1041,10 @@
         </is>
       </c>
       <c r="C42" s="3" t="n">
-        <v>1326.34</v>
+        <v>1325.78</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>1500</v>
+        <v>1470.47</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="F42" s="4" t="n">
-        <v>0.3955549509245275</v>
+        <v>0.4360382848393158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Elo Decimal Place Inconsistencies
</commit_message>
<xml_diff>
--- a/nba_elo_tracker.xlsx
+++ b/nba_elo_tracker.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.############"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.##"/>
+    <numFmt numFmtId="165" formatCode="0.############"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -80,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -88,6 +89,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -530,8 +534,10 @@
           <t>Cleveland Cavaliers</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
-        <v>1797.1</v>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>1797.11</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -543,8 +549,10 @@
           <t>Oklahoma City Thunder</t>
         </is>
       </c>
-      <c r="C6" s="3" t="n">
-        <v>1777.48</v>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>1777.48</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -556,8 +564,10 @@
           <t>Boston Celtics</t>
         </is>
       </c>
-      <c r="C7" s="3" t="n">
-        <v>1683.9</v>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>1683.89</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -569,8 +579,10 @@
           <t>Denver Nuggets</t>
         </is>
       </c>
-      <c r="C8" s="3" t="n">
-        <v>1661.8</v>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>1661.8</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -582,8 +594,10 @@
           <t>New York Knicks</t>
         </is>
       </c>
-      <c r="C9" s="3" t="n">
-        <v>1616.82</v>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>1616.82</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -595,8 +609,10 @@
           <t>Memphis Grizzlies</t>
         </is>
       </c>
-      <c r="C10" s="3" t="n">
-        <v>1612.74</v>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>1612.74</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -608,8 +624,10 @@
           <t>Los Angeles Lakers</t>
         </is>
       </c>
-      <c r="C11" s="3" t="n">
-        <v>1601.3</v>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>1601.3</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -621,8 +639,10 @@
           <t>Golden State Warriors</t>
         </is>
       </c>
-      <c r="C12" s="3" t="n">
-        <v>1589.98</v>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>1589.98</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -634,8 +654,10 @@
           <t>Minnesota Timberwolves</t>
         </is>
       </c>
-      <c r="C13" s="3" t="n">
-        <v>1588.03</v>
+      <c r="C13" s="4" t="inlineStr">
+        <is>
+          <t>1588.03</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -647,8 +669,10 @@
           <t>Houston Rockets</t>
         </is>
       </c>
-      <c r="C14" s="3" t="n">
-        <v>1582.82</v>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>1582.82</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -660,8 +684,10 @@
           <t>Detroit Pistons</t>
         </is>
       </c>
-      <c r="C15" s="3" t="n">
-        <v>1578.14</v>
+      <c r="C15" s="4" t="inlineStr">
+        <is>
+          <t>1578.14</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -673,8 +699,10 @@
           <t>Indiana Pacers</t>
         </is>
       </c>
-      <c r="C16" s="3" t="n">
-        <v>1551.64</v>
+      <c r="C16" s="4" t="inlineStr">
+        <is>
+          <t>1551.64</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -686,8 +714,10 @@
           <t>Milwaukee Bucks</t>
         </is>
       </c>
-      <c r="C17" s="3" t="n">
-        <v>1541.98</v>
+      <c r="C17" s="4" t="inlineStr">
+        <is>
+          <t>1541.99</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -699,8 +729,10 @@
           <t>Sacramento Kings</t>
         </is>
       </c>
-      <c r="C18" s="3" t="n">
-        <v>1529.16</v>
+      <c r="C18" s="4" t="inlineStr">
+        <is>
+          <t>1529.16</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -712,8 +744,10 @@
           <t>Atlanta Hawks</t>
         </is>
       </c>
-      <c r="C19" s="3" t="n">
-        <v>1502.88</v>
+      <c r="C19" s="4" t="inlineStr">
+        <is>
+          <t>1502.88</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -725,8 +759,10 @@
           <t>Dallas Mavericks</t>
         </is>
       </c>
-      <c r="C20" s="3" t="n">
-        <v>1478.74</v>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>1478.74</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -738,8 +774,10 @@
           <t>Los Angeles Clippers</t>
         </is>
       </c>
-      <c r="C21" s="3" t="n">
-        <v>1470.47</v>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>1470.47</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -751,8 +789,10 @@
           <t>Portland Trail Blazers</t>
         </is>
       </c>
-      <c r="C22" s="3" t="n">
-        <v>1465.62</v>
+      <c r="C22" s="4" t="inlineStr">
+        <is>
+          <t>1465.62</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -764,8 +804,10 @@
           <t>Chicago Bulls</t>
         </is>
       </c>
-      <c r="C23" s="3" t="n">
-        <v>1438.25</v>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
+          <t>1438.25</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -777,8 +819,10 @@
           <t>Miami Heat</t>
         </is>
       </c>
-      <c r="C24" s="3" t="n">
-        <v>1438.01</v>
+      <c r="C24" s="4" t="inlineStr">
+        <is>
+          <t>1438.0</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -790,8 +834,10 @@
           <t>Phoenix Suns</t>
         </is>
       </c>
-      <c r="C25" s="3" t="n">
-        <v>1436.24</v>
+      <c r="C25" s="4" t="inlineStr">
+        <is>
+          <t>1436.24</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -803,8 +849,10 @@
           <t>San Antonio Spurs</t>
         </is>
       </c>
-      <c r="C26" s="3" t="n">
-        <v>1409.99</v>
+      <c r="C26" s="4" t="inlineStr">
+        <is>
+          <t>1409.99</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -816,8 +864,10 @@
           <t>Orlando Magic</t>
         </is>
       </c>
-      <c r="C27" s="3" t="n">
-        <v>1388.17</v>
+      <c r="C27" s="4" t="inlineStr">
+        <is>
+          <t>1388.17</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -829,8 +879,10 @@
           <t>Toronto Raptors</t>
         </is>
       </c>
-      <c r="C28" s="3" t="n">
-        <v>1378.24</v>
+      <c r="C28" s="4" t="inlineStr">
+        <is>
+          <t>1378.24</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -842,8 +894,10 @@
           <t>Philadelphia 76ers</t>
         </is>
       </c>
-      <c r="C29" s="3" t="n">
-        <v>1358.1</v>
+      <c r="C29" s="4" t="inlineStr">
+        <is>
+          <t>1358.1</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -855,8 +909,10 @@
           <t>Brooklyn Nets</t>
         </is>
       </c>
-      <c r="C30" s="3" t="n">
-        <v>1355.48</v>
+      <c r="C30" s="4" t="inlineStr">
+        <is>
+          <t>1355.48</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -868,8 +924,10 @@
           <t>New Orleans Pelicans</t>
         </is>
       </c>
-      <c r="C31" s="3" t="n">
-        <v>1325.78</v>
+      <c r="C31" s="4" t="inlineStr">
+        <is>
+          <t>1325.78</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -881,8 +939,10 @@
           <t>Utah Jazz</t>
         </is>
       </c>
-      <c r="C32" s="3" t="n">
-        <v>1285.63</v>
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>1285.63</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -894,8 +954,10 @@
           <t>Washington Wizards</t>
         </is>
       </c>
-      <c r="C33" s="3" t="n">
-        <v>1277.19</v>
+      <c r="C33" s="4" t="inlineStr">
+        <is>
+          <t>1277.19</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -907,8 +969,10 @@
           <t>Charlotte Hornets</t>
         </is>
       </c>
-      <c r="C34" s="3" t="n">
-        <v>1262.75</v>
+      <c r="C34" s="4" t="inlineStr">
+        <is>
+          <t>1262.75</t>
+        </is>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1"/>
@@ -962,19 +1026,25 @@
           <t>Brooklyn Nets</t>
         </is>
       </c>
-      <c r="C39" s="3" t="n">
-        <v>1797.1</v>
-      </c>
-      <c r="D39" s="3" t="n">
-        <v>1355.48</v>
+      <c r="C39" s="4" t="inlineStr">
+        <is>
+          <t>1797.11</t>
+        </is>
+      </c>
+      <c r="D39" s="4" t="inlineStr">
+        <is>
+          <t>1355.48</t>
+        </is>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
           <t>Cleveland Cavaliers</t>
         </is>
       </c>
-      <c r="F39" s="4" t="n">
-        <v>0.9576216581651262</v>
+      <c r="F39" s="5" t="inlineStr">
+        <is>
+          <t>0.9576239942153544</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -988,19 +1058,25 @@
           <t>Washington Wizards</t>
         </is>
       </c>
-      <c r="C40" s="3" t="n">
-        <v>1578.14</v>
-      </c>
-      <c r="D40" s="3" t="n">
-        <v>1277.19</v>
+      <c r="C40" s="4" t="inlineStr">
+        <is>
+          <t>1578.14</t>
+        </is>
+      </c>
+      <c r="D40" s="4" t="inlineStr">
+        <is>
+          <t>1277.19</t>
+        </is>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
           <t>Detroit Pistons</t>
         </is>
       </c>
-      <c r="F40" s="4" t="n">
-        <v>0.9095418528145847</v>
+      <c r="F40" s="5" t="inlineStr">
+        <is>
+          <t>0.9095418528145847</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1014,19 +1090,25 @@
           <t>Milwaukee Bucks</t>
         </is>
       </c>
-      <c r="C41" s="3" t="n">
-        <v>1551.64</v>
-      </c>
-      <c r="D41" s="3" t="n">
-        <v>1541.98</v>
+      <c r="C41" s="4" t="inlineStr">
+        <is>
+          <t>1551.64</t>
+        </is>
+      </c>
+      <c r="D41" s="4" t="inlineStr">
+        <is>
+          <t>1541.99</t>
+        </is>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
           <t>Indiana Pacers</t>
         </is>
       </c>
-      <c r="F41" s="4" t="n">
-        <v>0.6527736812238141</v>
+      <c r="F41" s="5" t="inlineStr">
+        <is>
+          <t>0.652760633498995</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -1040,19 +1122,25 @@
           <t>Los Angeles Clippers</t>
         </is>
       </c>
-      <c r="C42" s="3" t="n">
-        <v>1325.78</v>
-      </c>
-      <c r="D42" s="3" t="n">
-        <v>1470.47</v>
+      <c r="C42" s="4" t="inlineStr">
+        <is>
+          <t>1325.78</t>
+        </is>
+      </c>
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>1470.47</t>
+        </is>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
           <t>Los Angeles Clippers</t>
         </is>
       </c>
-      <c r="F42" s="4" t="n">
-        <v>0.4360382848393158</v>
+      <c r="F42" s="5" t="inlineStr">
+        <is>
+          <t>0.4360382848393158</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>